<commit_message>
meaning preservation datasets implemented, questeval dataset implemented
</commit_message>
<xml_diff>
--- a/workspace/datasets/English_Datasets.xlsx
+++ b/workspace/datasets/English_Datasets.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christin/Desktop/USB-Pipeline/workspace/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A39BD5A-29D3-194D-8EE4-42BDD15AF891}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24392ED1-2CC8-C345-96C4-57E17C3E6E8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1080" windowWidth="28800" windowHeight="16280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabellenblatt1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="77">
   <si>
     <t>ds_id</t>
   </si>
@@ -248,6 +248,9 @@
   </si>
   <si>
     <t>britannica</t>
+  </si>
+  <si>
+    <t>QuestEval</t>
   </si>
 </sst>
 </file>
@@ -791,7 +794,7 @@
   <dimension ref="A1:AR999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A17" sqref="A17:D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1862,16 +1865,16 @@
     </row>
     <row r="17" spans="1:44" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="4" t="s">
-        <v>54</v>
+        <v>76</v>
       </c>
-      <c r="B17" s="3">
-        <v>2007</v>
+      <c r="B17" s="2">
+        <v>2021</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="11" t="s">
-        <v>20</v>
+      <c r="D17" s="4" t="s">
+        <v>12</v>
       </c>
       <c r="E17" s="3">
         <v>0</v>
@@ -1928,16 +1931,16 @@
     </row>
     <row r="18" spans="1:44" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
-      <c r="B18" s="2">
-        <v>2016</v>
+      <c r="B18" s="3">
+        <v>2007</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>57</v>
+        <v>11</v>
       </c>
-      <c r="D18" s="4" t="s">
-        <v>58</v>
+      <c r="D18" s="11" t="s">
+        <v>20</v>
       </c>
       <c r="E18" s="2">
         <v>0</v>
@@ -1994,16 +1997,16 @@
     </row>
     <row r="19" spans="1:44" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="4" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B19" s="2">
-        <v>2022</v>
+        <v>2016</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>11</v>
+        <v>57</v>
       </c>
-      <c r="D19" s="5" t="s">
-        <v>12</v>
+      <c r="D19" s="4" t="s">
+        <v>58</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>13</v>
@@ -2049,14 +2052,14 @@
       <c r="AR19" s="3"/>
     </row>
     <row r="20" spans="1:44" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="3" t="s">
-        <v>61</v>
+      <c r="A20" s="4" t="s">
+        <v>60</v>
       </c>
       <c r="B20" s="2">
-        <v>2016</v>
+        <v>2022</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>12</v>
@@ -2116,7 +2119,7 @@
     </row>
     <row r="21" spans="1:44" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B21" s="2">
         <v>2016</v>
@@ -2182,13 +2185,13 @@
     </row>
     <row r="22" spans="1:44" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
-      <c r="B22" s="26">
-        <v>2020</v>
+      <c r="B22" s="2">
+        <v>2016</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>12</v>
@@ -2248,7 +2251,7 @@
     </row>
     <row r="23" spans="1:44" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B23" s="26">
         <v>2020</v>
@@ -2313,14 +2316,14 @@
       <c r="AR23" s="3"/>
     </row>
     <row r="24" spans="1:44" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="2" t="s">
-        <v>69</v>
+      <c r="A24" s="3" t="s">
+        <v>68</v>
       </c>
-      <c r="B24" s="2">
-        <v>2011</v>
+      <c r="B24" s="26">
+        <v>2020</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>12</v>
@@ -2380,10 +2383,10 @@
     </row>
     <row r="25" spans="1:44" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B25" s="2">
-        <v>2013</v>
+        <v>2011</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>26</v>
@@ -2445,14 +2448,14 @@
       <c r="AR25" s="3"/>
     </row>
     <row r="26" spans="1:44" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="3" t="s">
-        <v>72</v>
+      <c r="A26" s="2" t="s">
+        <v>71</v>
       </c>
-      <c r="B26" s="3">
-        <v>2018</v>
+      <c r="B26" s="2">
+        <v>2013</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>12</v>
@@ -2511,50 +2514,18 @@
       <c r="AR26" s="3"/>
     </row>
     <row r="27" spans="1:44" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="4"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
-      <c r="J27" s="2"/>
-      <c r="K27" s="2"/>
-      <c r="L27" s="2"/>
-      <c r="M27" s="2"/>
-      <c r="N27" s="7"/>
-      <c r="O27" s="31"/>
-      <c r="P27" s="4"/>
-      <c r="Q27" s="9"/>
-      <c r="R27" s="4"/>
-      <c r="S27" s="4"/>
-      <c r="T27" s="4"/>
-      <c r="U27" s="4"/>
-      <c r="V27" s="4"/>
-      <c r="W27" s="4"/>
-      <c r="X27" s="2"/>
-      <c r="Y27" s="4"/>
-      <c r="Z27" s="4"/>
-      <c r="AA27" s="31"/>
-      <c r="AB27" s="3"/>
-      <c r="AC27" s="3"/>
-      <c r="AD27" s="3"/>
-      <c r="AE27" s="3"/>
-      <c r="AF27" s="3"/>
-      <c r="AG27" s="3"/>
-      <c r="AH27" s="3"/>
-      <c r="AI27" s="3"/>
-      <c r="AJ27" s="3"/>
-      <c r="AK27" s="3"/>
-      <c r="AL27" s="3"/>
-      <c r="AM27" s="3"/>
-      <c r="AN27" s="3"/>
-      <c r="AO27" s="3"/>
-      <c r="AP27" s="3"/>
-      <c r="AQ27" s="3"/>
-      <c r="AR27" s="3"/>
+      <c r="A27" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B27" s="3">
+        <v>2018</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="28" spans="1:44" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="4"/>
@@ -2695,10 +2666,6 @@
       <c r="AR30" s="3"/>
     </row>
     <row r="31" spans="1:44" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="4"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
       <c r="E31" s="2"/>
       <c r="F31" s="4"/>
       <c r="G31" s="4"/>
@@ -47285,15 +47252,15 @@
     <hyperlink ref="J14" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
     <hyperlink ref="J15" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
     <hyperlink ref="J16" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="J17" r:id="rId16" location="data" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="J18" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="J20" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="J21" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="J22" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="J23" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="J24" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="J25" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="J26" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="J18" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="J20" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="J21" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="J22" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="J23" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="J24" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="J25" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="J26" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="J17" r:id="rId24" location="data" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>